<commit_message>
working test iterations and test matrices
</commit_message>
<xml_diff>
--- a/results/test/1/1_test_stats.xlsx
+++ b/results/test/1/1_test_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="18">
   <si>
     <t>Game_num</t>
   </si>
@@ -49,25 +49,25 @@
     <t>Avg Dist</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>B</t>
   </si>
   <si>
-    <t>A</t>
+    <t>C</t>
   </si>
   <si>
     <t>D</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>1: action-distribution, positive rewards</t>
   </si>
   <si>
-    <t>Seq3</t>
+    <t>Custom</t>
   </si>
   <si>
-    <t>BADCDCBDABCBABADCDCBCBCBACBADADADCDABADADCBCBCDA</t>
+    <t>ABCADBCAABCADBCAABCADBCAABCADBCAABCADBCAABCADBCAABCADBCAABCADBCAABCADBCAABCADBCA</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,10 +486,10 @@
         <v>17</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H2">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -498,10 +498,10 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L2">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -524,10 +524,10 @@
         <v>17</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H3">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -536,10 +536,10 @@
         <v>2</v>
       </c>
       <c r="K3">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L3">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -562,22 +562,22 @@
         <v>17</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L4">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -588,7 +588,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -600,22 +600,22 @@
         <v>17</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L5">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -626,7 +626,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -638,22 +638,22 @@
         <v>17</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H6">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L6">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -664,7 +664,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -676,22 +676,22 @@
         <v>17</v>
       </c>
       <c r="G7">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L7">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -702,7 +702,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -714,22 +714,22 @@
         <v>17</v>
       </c>
       <c r="G8">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H8">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L8">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -740,7 +740,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -752,22 +752,22 @@
         <v>17</v>
       </c>
       <c r="G9">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H9">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J9">
         <v>2</v>
       </c>
       <c r="K9">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L9">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -778,7 +778,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -790,22 +790,22 @@
         <v>17</v>
       </c>
       <c r="G10">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L10">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -816,7 +816,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -828,22 +828,22 @@
         <v>17</v>
       </c>
       <c r="G11">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H11">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L11">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -854,7 +854,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -866,22 +866,22 @@
         <v>17</v>
       </c>
       <c r="G12">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L12">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -904,22 +904,22 @@
         <v>17</v>
       </c>
       <c r="G13">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H13">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K13">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L13">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -930,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -942,22 +942,22 @@
         <v>17</v>
       </c>
       <c r="G14">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H14">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K14">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L14">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -968,7 +968,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
@@ -980,22 +980,22 @@
         <v>17</v>
       </c>
       <c r="G15">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H15">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L15">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1006,7 +1006,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
@@ -1018,22 +1018,22 @@
         <v>17</v>
       </c>
       <c r="G16">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H16">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L16">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1044,7 +1044,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -1056,22 +1056,22 @@
         <v>17</v>
       </c>
       <c r="G17">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H17">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L17">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1082,7 +1082,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
@@ -1094,22 +1094,22 @@
         <v>17</v>
       </c>
       <c r="G18">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H18">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L18">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1120,7 +1120,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -1132,22 +1132,22 @@
         <v>17</v>
       </c>
       <c r="G19">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H19">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K19">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L19">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1158,7 +1158,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -1170,22 +1170,22 @@
         <v>17</v>
       </c>
       <c r="G20">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H20">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L20">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1208,22 +1208,22 @@
         <v>17</v>
       </c>
       <c r="G21">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H21">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K21">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L21">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1246,22 +1246,22 @@
         <v>17</v>
       </c>
       <c r="G22">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H22">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K22">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L22">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1272,7 +1272,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
@@ -1284,22 +1284,22 @@
         <v>17</v>
       </c>
       <c r="G23">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H23">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K23">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L23">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1310,7 +1310,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
@@ -1322,22 +1322,22 @@
         <v>17</v>
       </c>
       <c r="G24">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H24">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K24">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L24">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1360,22 +1360,22 @@
         <v>17</v>
       </c>
       <c r="G25">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H25">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K25">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L25">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1386,7 +1386,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
@@ -1398,22 +1398,22 @@
         <v>17</v>
       </c>
       <c r="G26">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K26">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L26">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1424,7 +1424,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
@@ -1436,22 +1436,22 @@
         <v>17</v>
       </c>
       <c r="G27">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H27">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K27">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L27">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1462,7 +1462,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
@@ -1474,22 +1474,22 @@
         <v>17</v>
       </c>
       <c r="G28">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H28">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K28">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L28">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1500,7 +1500,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
         <v>15</v>
@@ -1512,22 +1512,22 @@
         <v>17</v>
       </c>
       <c r="G29">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H29">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K29">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L29">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1538,7 +1538,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
         <v>15</v>
@@ -1550,22 +1550,22 @@
         <v>17</v>
       </c>
       <c r="G30">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H30">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I30">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K30">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L30">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1588,22 +1588,22 @@
         <v>17</v>
       </c>
       <c r="G31">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H31">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K31">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L31">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1626,22 +1626,22 @@
         <v>17</v>
       </c>
       <c r="G32">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H32">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K32">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L32">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1652,7 +1652,7 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33" t="s">
         <v>15</v>
@@ -1664,22 +1664,22 @@
         <v>17</v>
       </c>
       <c r="G33">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H33">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K33">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L33">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1690,7 +1690,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -1702,22 +1702,22 @@
         <v>17</v>
       </c>
       <c r="G34">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H34">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K34">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L34">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1728,7 +1728,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
@@ -1740,22 +1740,22 @@
         <v>17</v>
       </c>
       <c r="G35">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H35">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I35">
         <v>4</v>
       </c>
       <c r="J35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K35">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L35">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1778,22 +1778,22 @@
         <v>17</v>
       </c>
       <c r="G36">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H36">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K36">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L36">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1804,7 +1804,7 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -1816,22 +1816,22 @@
         <v>17</v>
       </c>
       <c r="G37">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H37">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K37">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L37">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1842,7 +1842,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -1854,22 +1854,22 @@
         <v>17</v>
       </c>
       <c r="G38">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H38">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K38">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L38">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -1892,22 +1892,22 @@
         <v>17</v>
       </c>
       <c r="G39">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H39">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K39">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L39">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1930,22 +1930,22 @@
         <v>17</v>
       </c>
       <c r="G40">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H40">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K40">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L40">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -1956,7 +1956,7 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
@@ -1968,22 +1968,22 @@
         <v>17</v>
       </c>
       <c r="G41">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H41">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I41">
         <v>2</v>
       </c>
       <c r="J41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K41">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L41">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -1994,7 +1994,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
         <v>15</v>
@@ -2006,22 +2006,22 @@
         <v>17</v>
       </c>
       <c r="G42">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H42">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K42">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L42">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2032,7 +2032,7 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
         <v>15</v>
@@ -2044,22 +2044,22 @@
         <v>17</v>
       </c>
       <c r="G43">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H43">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I43">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J43">
         <v>3</v>
       </c>
       <c r="K43">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L43">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2070,7 +2070,7 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
         <v>15</v>
@@ -2082,10 +2082,10 @@
         <v>17</v>
       </c>
       <c r="G44">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H44">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I44">
         <v>2</v>
@@ -2094,10 +2094,10 @@
         <v>2</v>
       </c>
       <c r="K44">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L44">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2108,7 +2108,7 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D45" t="s">
         <v>15</v>
@@ -2120,22 +2120,22 @@
         <v>17</v>
       </c>
       <c r="G45">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H45">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K45">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L45">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2146,7 +2146,7 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D46" t="s">
         <v>15</v>
@@ -2158,22 +2158,22 @@
         <v>17</v>
       </c>
       <c r="G46">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H46">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I46">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K46">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L46">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2184,7 +2184,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D47" t="s">
         <v>15</v>
@@ -2196,22 +2196,22 @@
         <v>17</v>
       </c>
       <c r="G47">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H47">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K47">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L47">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -2234,22 +2234,22 @@
         <v>17</v>
       </c>
       <c r="G48">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H48">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K48">
-        <v>2.395833333333333</v>
+        <v>2.0375</v>
       </c>
       <c r="L48">
-        <v>2.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -2260,34 +2260,1250 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49">
+        <v>1000</v>
+      </c>
+      <c r="H49">
+        <v>5</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>2.0375</v>
+      </c>
+      <c r="L49">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" t="s">
+        <v>17</v>
+      </c>
+      <c r="G50">
+        <v>1000</v>
+      </c>
+      <c r="H50">
+        <v>5</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>2.0375</v>
+      </c>
+      <c r="L50">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
         <v>12</v>
       </c>
-      <c r="D49" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" t="s">
-        <v>17</v>
-      </c>
-      <c r="G49">
-        <v>100</v>
-      </c>
-      <c r="H49">
-        <v>20</v>
-      </c>
-      <c r="I49">
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" t="s">
+        <v>17</v>
+      </c>
+      <c r="G51">
+        <v>1000</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>4</v>
+      </c>
+      <c r="J51">
+        <v>3</v>
+      </c>
+      <c r="K51">
+        <v>2.0375</v>
+      </c>
+      <c r="L51">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" t="s">
+        <v>17</v>
+      </c>
+      <c r="G52">
+        <v>1000</v>
+      </c>
+      <c r="H52">
+        <v>5</v>
+      </c>
+      <c r="I52">
         <v>2</v>
       </c>
-      <c r="J49">
+      <c r="J52">
         <v>2</v>
       </c>
-      <c r="K49">
-        <v>2.395833333333333</v>
-      </c>
-      <c r="L49">
-        <v>2.25</v>
+      <c r="K52">
+        <v>2.0375</v>
+      </c>
+      <c r="L52">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53">
+        <v>1000</v>
+      </c>
+      <c r="H53">
+        <v>5</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>2.0375</v>
+      </c>
+      <c r="L53">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54">
+        <v>1000</v>
+      </c>
+      <c r="H54">
+        <v>5</v>
+      </c>
+      <c r="I54">
+        <v>4</v>
+      </c>
+      <c r="J54">
+        <v>4</v>
+      </c>
+      <c r="K54">
+        <v>2.0375</v>
+      </c>
+      <c r="L54">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" t="s">
+        <v>17</v>
+      </c>
+      <c r="G55">
+        <v>1000</v>
+      </c>
+      <c r="H55">
+        <v>5</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>2.0375</v>
+      </c>
+      <c r="L55">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56">
+        <v>1000</v>
+      </c>
+      <c r="H56">
+        <v>5</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>2.0375</v>
+      </c>
+      <c r="L56">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" t="s">
+        <v>17</v>
+      </c>
+      <c r="G57">
+        <v>1000</v>
+      </c>
+      <c r="H57">
+        <v>5</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>2.0375</v>
+      </c>
+      <c r="L57">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" t="s">
+        <v>17</v>
+      </c>
+      <c r="G58">
+        <v>1000</v>
+      </c>
+      <c r="H58">
+        <v>5</v>
+      </c>
+      <c r="I58">
+        <v>17</v>
+      </c>
+      <c r="J58">
+        <v>3</v>
+      </c>
+      <c r="K58">
+        <v>2.0375</v>
+      </c>
+      <c r="L58">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" t="s">
+        <v>17</v>
+      </c>
+      <c r="G59">
+        <v>1000</v>
+      </c>
+      <c r="H59">
+        <v>5</v>
+      </c>
+      <c r="I59">
+        <v>3</v>
+      </c>
+      <c r="J59">
+        <v>3</v>
+      </c>
+      <c r="K59">
+        <v>2.0375</v>
+      </c>
+      <c r="L59">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60">
+        <v>1000</v>
+      </c>
+      <c r="H60">
+        <v>5</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <v>2.0375</v>
+      </c>
+      <c r="L60">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61">
+        <v>1000</v>
+      </c>
+      <c r="H61">
+        <v>5</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>2.0375</v>
+      </c>
+      <c r="L61">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" t="s">
+        <v>17</v>
+      </c>
+      <c r="G62">
+        <v>1000</v>
+      </c>
+      <c r="H62">
+        <v>5</v>
+      </c>
+      <c r="I62">
+        <v>5</v>
+      </c>
+      <c r="J62">
+        <v>4</v>
+      </c>
+      <c r="K62">
+        <v>2.0375</v>
+      </c>
+      <c r="L62">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G63">
+        <v>1000</v>
+      </c>
+      <c r="H63">
+        <v>5</v>
+      </c>
+      <c r="I63">
+        <v>2</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+      <c r="K63">
+        <v>2.0375</v>
+      </c>
+      <c r="L63">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" t="s">
+        <v>16</v>
+      </c>
+      <c r="F64" t="s">
+        <v>17</v>
+      </c>
+      <c r="G64">
+        <v>1000</v>
+      </c>
+      <c r="H64">
+        <v>5</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>2.0375</v>
+      </c>
+      <c r="L64">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65">
+        <v>1000</v>
+      </c>
+      <c r="H65">
+        <v>5</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <v>2.0375</v>
+      </c>
+      <c r="L65">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" t="s">
+        <v>17</v>
+      </c>
+      <c r="G66">
+        <v>1000</v>
+      </c>
+      <c r="H66">
+        <v>5</v>
+      </c>
+      <c r="I66">
+        <v>4</v>
+      </c>
+      <c r="J66">
+        <v>3</v>
+      </c>
+      <c r="K66">
+        <v>2.0375</v>
+      </c>
+      <c r="L66">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" t="s">
+        <v>16</v>
+      </c>
+      <c r="F67" t="s">
+        <v>17</v>
+      </c>
+      <c r="G67">
+        <v>1000</v>
+      </c>
+      <c r="H67">
+        <v>5</v>
+      </c>
+      <c r="I67">
+        <v>3</v>
+      </c>
+      <c r="J67">
+        <v>3</v>
+      </c>
+      <c r="K67">
+        <v>2.0375</v>
+      </c>
+      <c r="L67">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" t="s">
+        <v>16</v>
+      </c>
+      <c r="F68" t="s">
+        <v>17</v>
+      </c>
+      <c r="G68">
+        <v>1000</v>
+      </c>
+      <c r="H68">
+        <v>5</v>
+      </c>
+      <c r="I68">
+        <v>5</v>
+      </c>
+      <c r="J68">
+        <v>3</v>
+      </c>
+      <c r="K68">
+        <v>2.0375</v>
+      </c>
+      <c r="L68">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69" t="s">
+        <v>17</v>
+      </c>
+      <c r="G69">
+        <v>1000</v>
+      </c>
+      <c r="H69">
+        <v>5</v>
+      </c>
+      <c r="I69">
+        <v>3</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>2.0375</v>
+      </c>
+      <c r="L69">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" t="s">
+        <v>16</v>
+      </c>
+      <c r="F70" t="s">
+        <v>17</v>
+      </c>
+      <c r="G70">
+        <v>1000</v>
+      </c>
+      <c r="H70">
+        <v>5</v>
+      </c>
+      <c r="I70">
+        <v>5</v>
+      </c>
+      <c r="J70">
+        <v>4</v>
+      </c>
+      <c r="K70">
+        <v>2.0375</v>
+      </c>
+      <c r="L70">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" t="s">
+        <v>16</v>
+      </c>
+      <c r="F71" t="s">
+        <v>17</v>
+      </c>
+      <c r="G71">
+        <v>1000</v>
+      </c>
+      <c r="H71">
+        <v>5</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>2.0375</v>
+      </c>
+      <c r="L71">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" t="s">
+        <v>16</v>
+      </c>
+      <c r="F72" t="s">
+        <v>17</v>
+      </c>
+      <c r="G72">
+        <v>1000</v>
+      </c>
+      <c r="H72">
+        <v>5</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>2.0375</v>
+      </c>
+      <c r="L72">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" t="s">
+        <v>16</v>
+      </c>
+      <c r="F73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G73">
+        <v>1000</v>
+      </c>
+      <c r="H73">
+        <v>5</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <v>2.0375</v>
+      </c>
+      <c r="L73">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" t="s">
+        <v>15</v>
+      </c>
+      <c r="E74" t="s">
+        <v>16</v>
+      </c>
+      <c r="F74" t="s">
+        <v>17</v>
+      </c>
+      <c r="G74">
+        <v>1000</v>
+      </c>
+      <c r="H74">
+        <v>5</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>2.0375</v>
+      </c>
+      <c r="L74">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" t="s">
+        <v>17</v>
+      </c>
+      <c r="G75">
+        <v>1000</v>
+      </c>
+      <c r="H75">
+        <v>5</v>
+      </c>
+      <c r="I75">
+        <v>6</v>
+      </c>
+      <c r="J75">
+        <v>4</v>
+      </c>
+      <c r="K75">
+        <v>2.0375</v>
+      </c>
+      <c r="L75">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" t="s">
+        <v>16</v>
+      </c>
+      <c r="F76" t="s">
+        <v>17</v>
+      </c>
+      <c r="G76">
+        <v>1000</v>
+      </c>
+      <c r="H76">
+        <v>5</v>
+      </c>
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>2.0375</v>
+      </c>
+      <c r="L76">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" t="s">
+        <v>15</v>
+      </c>
+      <c r="E77" t="s">
+        <v>16</v>
+      </c>
+      <c r="F77" t="s">
+        <v>17</v>
+      </c>
+      <c r="G77">
+        <v>1000</v>
+      </c>
+      <c r="H77">
+        <v>5</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
+        <v>2.0375</v>
+      </c>
+      <c r="L77">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s">
+        <v>15</v>
+      </c>
+      <c r="E78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F78" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78">
+        <v>1000</v>
+      </c>
+      <c r="H78">
+        <v>5</v>
+      </c>
+      <c r="I78">
+        <v>4</v>
+      </c>
+      <c r="J78">
+        <v>4</v>
+      </c>
+      <c r="K78">
+        <v>2.0375</v>
+      </c>
+      <c r="L78">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" t="s">
+        <v>15</v>
+      </c>
+      <c r="E79" t="s">
+        <v>16</v>
+      </c>
+      <c r="F79" t="s">
+        <v>17</v>
+      </c>
+      <c r="G79">
+        <v>1000</v>
+      </c>
+      <c r="H79">
+        <v>5</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>2.0375</v>
+      </c>
+      <c r="L79">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80" t="s">
+        <v>13</v>
+      </c>
+      <c r="D80" t="s">
+        <v>15</v>
+      </c>
+      <c r="E80" t="s">
+        <v>16</v>
+      </c>
+      <c r="F80" t="s">
+        <v>17</v>
+      </c>
+      <c r="G80">
+        <v>1000</v>
+      </c>
+      <c r="H80">
+        <v>5</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>2.0375</v>
+      </c>
+      <c r="L80">
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" t="s">
+        <v>15</v>
+      </c>
+      <c r="E81" t="s">
+        <v>16</v>
+      </c>
+      <c r="F81" t="s">
+        <v>17</v>
+      </c>
+      <c r="G81">
+        <v>1000</v>
+      </c>
+      <c r="H81">
+        <v>5</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>2.0375</v>
+      </c>
+      <c r="L81">
+        <v>1.5625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>